<commit_message>
Created new page Confirm
</commit_message>
<xml_diff>
--- a/Documentos/CANVAS MVP.xlsx
+++ b/Documentos/CANVAS MVP.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3821145.UNIVALI\Documents\GitHub\legacyInfluencer\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wprojects\REACTNATIVE\legacyinfluencer\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,58 +38,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>FUNCIONALIDADES</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Cadastro de influenciadores digitais
-Cadastro de empresas
-Upload de imagens e vídeos
-Envio de notificações</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PROPOSTA DO MVP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Rede social voltada para contatos entre influenciadores digitais e empresas que desejam acompanhar e/ou contratar os serviços de influenciadores digitais.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>PERSONAS &amp; PLATAFORMAS</t>
     </r>
     <r>
@@ -210,11 +158,61 @@
 Projeto sem investimentos financeiros</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PROPOSTA DO MVP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Rede social voltada para contatos entre influenciadores digitais e empresas que desejam acompanhar e/ou contratar os serviços de influenciadores digitais.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FUNCIONALIDADES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Cadastro de influenciadores digitais
+Cadastro de empresas
+Envio de notificações</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -275,22 +273,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,66 +570,67 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:3" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>